<commit_message>
What is the Size of a Variable (sizeof)
</commit_message>
<xml_diff>
--- a/3.Variables-and-Constants/Variables-and-Constants.xlsx
+++ b/3.Variables-and-Constants/Variables-and-Constants.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\study\c-plus-plus\3.Variables-and-Constants\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F48868-4718-4683-9EEC-D18653DEE48B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3619741B-A43C-4554-9D7C-89DCA4B9311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31290" yWindow="1755" windowWidth="25500" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31290" yWindow="1755" windowWidth="25500" windowHeight="13440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Global Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="What is the Size of a Variable" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t>c-plus-plus</t>
     <phoneticPr fontId="1"/>
@@ -83,13 +84,266 @@
   </si>
   <si>
     <t xml:space="preserve">}       </t>
+  </si>
+  <si>
+    <t>2.What-is-the-Size-of-a-Variable</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SizeofOperator</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// Section 6</t>
+  </si>
+  <si>
+    <t>// The sizeof operator</t>
+  </si>
+  <si>
+    <t>#include &lt;climits&gt;      // make sure you include climits for integer types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  // Similar information for floating point numbers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  // is contained in &lt;cfloat&gt;</t>
+  </si>
+  <si>
+    <t>int main() {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "sizeof information" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "========================" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "char: " &lt;&lt; sizeof(char) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "int : " &lt;&lt; sizeof(int) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "unsigned int: " &lt;&lt; sizeof(unsigned int) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "short: " &lt;&lt; sizeof(short) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long: " &lt;&lt; sizeof(long) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long long: " &lt;&lt; sizeof(long long) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "float: " &lt;&lt; sizeof(float) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "double: " &lt;&lt; sizeof(double) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long double: " &lt;&lt; sizeof(long double) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // use values defined in &lt;climits&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Minimum values:" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "char: " &lt;&lt; CHAR_MIN &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "int: " &lt;&lt; INT_MIN &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "short: " &lt;&lt; SHRT_MIN &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long: " &lt;&lt; LONG_MIN &lt;&lt; endl; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long long: " &lt;&lt; LLONG_MIN &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "Maximum values:" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "char: " &lt;&lt; CHAR_MAX &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "int: " &lt;&lt; INT_MAX &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "short: " &lt;&lt; SHRT_MAX &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long: " &lt;&lt; LONG_MAX &lt;&lt; endl; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "long long: " &lt;&lt; LLONG_MAX &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">//    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // sizeof can also be used with variable names</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "sizeof using variable names" &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    int age {21};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    // or</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     cout &lt;&lt; "age is " &lt;&lt; sizeof age &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    double wage { 22.24};</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "wage is " &lt;&lt; sizeof(wage) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "wage is " &lt;&lt; sizeof wage &lt;&lt; " bytes." &lt;&lt; endl;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>ư</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ợ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>c đ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="163"/>
+      </rPr>
+      <t>ị</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Yu Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nh nghĩa bên ngoài hàm</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Sizeof can also be used to determine the sizeof compound types like arrays, structures and objects. In order to determine the sizeof a specific type, We can also determine the </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">sizeof variables using their names. </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>1 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>4 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>8 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>16 bytes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-9223372036854770000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>9223372036854775807</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→ the min value we can store in char type</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">    cout &lt;&lt; "age is " &lt;&lt; sizeof(age) &lt;&lt; " bytes." &lt;&lt; endl;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>→using sizeof with variable name</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -119,6 +373,27 @@
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Yu Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="163"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -221,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -234,6 +509,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -289,6 +566,55 @@
         <a:xfrm>
           <a:off x="733425" y="6730999"/>
           <a:ext cx="8877300" cy="2493199"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>93928</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="図 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56E2FD36-6C3C-5422-6B1C-F541C8119332}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="739775" y="19354800"/>
+          <a:ext cx="5327650" cy="6799528"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -565,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="S37" sqref="S37"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -663,130 +989,1170 @@
     </row>
     <row r="14" spans="2:9">
       <c r="B14" s="4"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="2:9">
       <c r="B15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
       <c r="F15" s="5"/>
     </row>
     <row r="16" spans="2:9">
       <c r="B16" s="4"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:8">
+      <c r="B17" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
       <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="G17" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8">
       <c r="B18" s="4"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:8">
       <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:8">
       <c r="B20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:8">
       <c r="B21" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:8">
       <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:8">
       <c r="B23" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
       <c r="F23" s="5"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:8">
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
       <c r="F24" s="5"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:8">
       <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
       <c r="F25" s="5"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:8">
       <c r="B26" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:8">
       <c r="B27" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
       <c r="F27" s="5"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:8">
       <c r="B28" s="8"/>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
       <c r="E28" s="9"/>
       <c r="F28" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BC5D08B-66ED-4366-B5FE-02D19159191E}">
+  <dimension ref="B3:L83"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="N66" sqref="N66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <cols>
+    <col min="11" max="11" width="14.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="4"/>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="4"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="4"/>
+      <c r="D7" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4"/>
+      <c r="D8" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="4"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="4"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="5"/>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="5"/>
+    </row>
+    <row r="24" spans="2:9">
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="5"/>
+    </row>
+    <row r="25" spans="2:9">
+      <c r="B25" s="4"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="11"/>
+      <c r="I25" s="5"/>
+    </row>
+    <row r="26" spans="2:9">
+      <c r="B26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="5"/>
+    </row>
+    <row r="27" spans="2:9">
+      <c r="B27" s="4"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="5"/>
+    </row>
+    <row r="28" spans="2:9">
+      <c r="B28" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="5"/>
+    </row>
+    <row r="29" spans="2:9">
+      <c r="B29" s="4"/>
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="2:9">
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="5"/>
+    </row>
+    <row r="31" spans="2:9">
+      <c r="B31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="5"/>
+    </row>
+    <row r="32" spans="2:9">
+      <c r="B32" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="5"/>
+      <c r="J33" t="s">
+        <v>66</v>
+      </c>
+      <c r="K33" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="5"/>
+      <c r="J34" t="s">
+        <v>66</v>
+      </c>
+      <c r="K34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11">
+      <c r="B35" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="5"/>
+      <c r="J35" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11">
+      <c r="B36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="5"/>
+      <c r="J36" t="s">
+        <v>66</v>
+      </c>
+      <c r="K36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="5"/>
+      <c r="J37" t="s">
+        <v>66</v>
+      </c>
+      <c r="K37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11">
+      <c r="B38" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="11"/>
+      <c r="I38" s="5"/>
+      <c r="J38" t="s">
+        <v>66</v>
+      </c>
+      <c r="K38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11">
+      <c r="B39" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="2:11">
+      <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="2:11">
+      <c r="B41" s="4"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="2:11">
+      <c r="B42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="5"/>
+      <c r="J42" t="s">
+        <v>66</v>
+      </c>
+      <c r="K42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11">
+      <c r="B43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="5"/>
+      <c r="J43" t="s">
+        <v>66</v>
+      </c>
+      <c r="K43" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11">
+      <c r="B44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="5"/>
+      <c r="J44" t="s">
+        <v>66</v>
+      </c>
+      <c r="K44" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11">
+      <c r="B45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="2:11">
+      <c r="B46" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="2:11">
+      <c r="B47" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="2:11">
+      <c r="B48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="2:12">
+      <c r="B49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="11"/>
+      <c r="D49" s="11"/>
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="11"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="2:12">
+      <c r="B50" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="H50" s="11"/>
+      <c r="I50" s="5"/>
+    </row>
+    <row r="51" spans="2:12">
+      <c r="B51" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="5"/>
+      <c r="J51" t="s">
+        <v>66</v>
+      </c>
+      <c r="K51">
+        <v>-128</v>
+      </c>
+      <c r="L51" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12">
+      <c r="B52" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="11"/>
+      <c r="D52" s="11"/>
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="5"/>
+      <c r="J52" t="s">
+        <v>66</v>
+      </c>
+      <c r="K52">
+        <v>-2147483648</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12">
+      <c r="B53" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="11"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="5"/>
+      <c r="J53" t="s">
+        <v>66</v>
+      </c>
+      <c r="K53">
+        <v>-32768</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12">
+      <c r="B54" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="11"/>
+      <c r="D54" s="11"/>
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="5"/>
+      <c r="J54" t="s">
+        <v>66</v>
+      </c>
+      <c r="K54">
+        <v>-2147483648</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12">
+      <c r="B55" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="D55" s="11"/>
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="5"/>
+      <c r="J55" t="s">
+        <v>66</v>
+      </c>
+      <c r="K55" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12">
+      <c r="B56" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C56" s="11"/>
+      <c r="D56" s="11"/>
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="5"/>
+    </row>
+    <row r="57" spans="2:12">
+      <c r="B57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C57" s="11"/>
+      <c r="D57" s="11"/>
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="5"/>
+    </row>
+    <row r="58" spans="2:12">
+      <c r="B58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C58" s="11"/>
+      <c r="D58" s="11"/>
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="5"/>
+    </row>
+    <row r="59" spans="2:12">
+      <c r="B59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="11"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="5"/>
+    </row>
+    <row r="60" spans="2:12">
+      <c r="B60" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C60" s="11"/>
+      <c r="D60" s="11"/>
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="5"/>
+      <c r="J60" t="s">
+        <v>66</v>
+      </c>
+      <c r="K60">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12">
+      <c r="B61" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="11"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="H61" s="11"/>
+      <c r="I61" s="5"/>
+      <c r="J61" t="s">
+        <v>66</v>
+      </c>
+      <c r="K61">
+        <v>2147483647</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12">
+      <c r="B62" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C62" s="11"/>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="5"/>
+      <c r="J62" t="s">
+        <v>66</v>
+      </c>
+      <c r="K62">
+        <v>32767</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12">
+      <c r="B63" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C63" s="11"/>
+      <c r="D63" s="11"/>
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+      <c r="I63" s="5"/>
+      <c r="J63" t="s">
+        <v>66</v>
+      </c>
+      <c r="K63">
+        <v>2147483647</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12">
+      <c r="B64" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" s="11"/>
+      <c r="D64" s="11"/>
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="H64" s="11"/>
+      <c r="I64" s="5"/>
+      <c r="J64" t="s">
+        <v>66</v>
+      </c>
+      <c r="K64" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="2:12">
+      <c r="B65" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C65" s="11"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="H65" s="11"/>
+      <c r="I65" s="5"/>
+    </row>
+    <row r="66" spans="2:12">
+      <c r="B66" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C66" s="11"/>
+      <c r="D66" s="11"/>
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="H66" s="11"/>
+      <c r="I66" s="5"/>
+    </row>
+    <row r="67" spans="2:12">
+      <c r="B67" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="11"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="11"/>
+      <c r="I67" s="5"/>
+    </row>
+    <row r="68" spans="2:12">
+      <c r="B68" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11"/>
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="11"/>
+      <c r="I68" s="5"/>
+    </row>
+    <row r="69" spans="2:12">
+      <c r="B69" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11"/>
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+      <c r="H69" s="11"/>
+      <c r="I69" s="5"/>
+    </row>
+    <row r="70" spans="2:12">
+      <c r="B70" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+      <c r="H70" s="11"/>
+      <c r="I70" s="5"/>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="11"/>
+      <c r="I71" s="5"/>
+      <c r="J71" t="s">
+        <v>66</v>
+      </c>
+      <c r="K71" t="s">
+        <v>68</v>
+      </c>
+      <c r="L71" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="72" spans="2:12">
+      <c r="B72" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" s="11"/>
+      <c r="D72" s="11"/>
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+      <c r="H72" s="11"/>
+      <c r="I72" s="5"/>
+    </row>
+    <row r="73" spans="2:12">
+      <c r="B73" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="11"/>
+      <c r="I73" s="5"/>
+      <c r="J73" t="s">
+        <v>66</v>
+      </c>
+      <c r="K73" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12">
+      <c r="B74" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11"/>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="11"/>
+      <c r="I74" s="5"/>
+    </row>
+    <row r="75" spans="2:12">
+      <c r="B75" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11"/>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="11"/>
+      <c r="I75" s="5"/>
+    </row>
+    <row r="76" spans="2:12">
+      <c r="B76" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11"/>
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+      <c r="H76" s="11"/>
+      <c r="I76" s="5"/>
+      <c r="J76" t="s">
+        <v>66</v>
+      </c>
+      <c r="K76" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="2:12">
+      <c r="B77" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C77" s="11"/>
+      <c r="D77" s="11"/>
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="11"/>
+      <c r="I77" s="5"/>
+    </row>
+    <row r="78" spans="2:12">
+      <c r="B78" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C78" s="11"/>
+      <c r="D78" s="11"/>
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+      <c r="H78" s="11"/>
+      <c r="I78" s="5"/>
+      <c r="J78" t="s">
+        <v>66</v>
+      </c>
+      <c r="K78" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="79" spans="2:12">
+      <c r="B79" s="4"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="11"/>
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="11"/>
+      <c r="I79" s="5"/>
+    </row>
+    <row r="80" spans="2:12">
+      <c r="B80" s="4"/>
+      <c r="C80" s="11"/>
+      <c r="D80" s="11"/>
+      <c r="E80" s="11"/>
+      <c r="F80" s="11"/>
+      <c r="G80" s="11"/>
+      <c r="H80" s="11"/>
+      <c r="I80" s="5"/>
+    </row>
+    <row r="81" spans="2:9">
+      <c r="B81" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11"/>
+      <c r="E81" s="11"/>
+      <c r="F81" s="11"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="11"/>
+      <c r="I81" s="5"/>
+    </row>
+    <row r="82" spans="2:9">
+      <c r="B82" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="11"/>
+      <c r="D82" s="11"/>
+      <c r="E82" s="11"/>
+      <c r="F82" s="11"/>
+      <c r="G82" s="11"/>
+      <c r="H82" s="11"/>
+      <c r="I82" s="5"/>
+    </row>
+    <row r="83" spans="2:9">
+      <c r="B83" s="8"/>
+      <c r="C83" s="9"/>
+      <c r="D83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
+      <c r="G83" s="9"/>
+      <c r="H83" s="9"/>
+      <c r="I83" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>